<commit_message>
ready for user acceptance test
</commit_message>
<xml_diff>
--- a/util/files/user.xlsx
+++ b/util/files/user.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B771C893-7C66-4090-8F40-5A530523F82F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674958DA-B745-454E-AA56-511E433EE535}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="1890" windowWidth="14400" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>espoir</t>
   </si>
@@ -24,16 +24,41 @@
   </si>
   <si>
     <t>Mbuyi</t>
+  </si>
+  <si>
+    <t>espoirditekemena@gmail.com</t>
+  </si>
+  <si>
+    <t>jds;oaiudisuygfoiu</t>
+  </si>
+  <si>
+    <t>Miriam</t>
+  </si>
+  <si>
+    <t>wa mbuyi</t>
+  </si>
+  <si>
+    <t>miriamMbuyi@gmail.com</t>
+  </si>
+  <si>
+    <t>jdhfdsfhjhffjdhdsj</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -55,13 +80,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -335,19 +363,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -357,8 +387,35 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1" xr:uid="{EF943DB0-F040-44FA-86DD-FF885A9BAD8D}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{B3D5A076-4B14-4549-B201-254BB98CB46E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>